<commit_message>
Import Error Bug Fixes for Advanced Stats
</commit_message>
<xml_diff>
--- a/2024NBAplayerStats.xlsx
+++ b/2024NBAplayerStats.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1017190F-48F0-48EC-9691-7FCBDD011382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8AB2F1-5A85-4EE9-9C19-8E928491C71C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="10755" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5303,7 +5303,7 @@
     <col min="15" max="16" width="4.54296875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="5.54296875" customWidth="1"/>
     <col min="18" max="18" width="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="2.76953125" customWidth="1"/>
     <col min="20" max="20" width="4.54296875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="5.54296875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="4.7265625" customWidth="1"/>

</xml_diff>